<commit_message>
power_consumption added, todo, jumpers_map R77 updated
</commit_message>
<xml_diff>
--- a/pcb/v1.1/jumpers_map.xlsx
+++ b/pcb/v1.1/jumpers_map.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\SocSys\auto_informer\autoinformer\pcb\v1.1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D3F1ED-C8B2-47E1-BAA4-D765B46F540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19275" yWindow="2535" windowWidth="17820" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19275" yWindow="2535" windowWidth="17820" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Позиционное обозначение</t>
   </si>
@@ -151,13 +145,22 @@
   </si>
   <si>
     <t>VT4, DA3</t>
+  </si>
+  <si>
+    <t>R77</t>
+  </si>
+  <si>
+    <t>Дополнительная нагрузка для STEP-UP DC-DC (LM2577)</t>
+  </si>
+  <si>
+    <t>TDA2003V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,7 +285,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -317,7 +320,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -494,29 +497,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:5" ht="32.25" customHeight="1" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -530,7 +533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="15.75" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -542,7 +545,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="15.75" thickBot="1">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -556,13 +559,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="15.75" thickBot="1">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="45.75" thickBot="1">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -576,7 +579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="30.75" thickBot="1">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -586,7 +589,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="15.75" thickBot="1">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
@@ -596,7 +599,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="15.75" thickBot="1">
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
@@ -608,7 +611,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="15.75" thickBot="1">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -622,7 +625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" ht="15.75" thickBot="1">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
@@ -634,7 +637,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="15.75" thickBot="1">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -648,7 +651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" ht="15.75" thickBot="1">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
@@ -660,7 +663,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" ht="15.75" thickBot="1">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -674,7 +677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" ht="15.75" thickBot="1">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -686,7 +689,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="15.75" thickBot="1">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
@@ -698,13 +701,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="15.75" thickBot="1">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="15.75" thickBot="1">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -716,7 +719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="15.75" thickBot="1">
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
@@ -728,7 +731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="15.75" thickBot="1">
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
@@ -740,13 +743,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="15.75" thickBot="1">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="30.75" thickBot="1">
       <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
@@ -758,25 +761,33 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="30.75" thickBot="1">
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" thickBot="1">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" ht="15.75" thickBot="1">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" ht="15.75" thickBot="1">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>

</xml_diff>

<commit_message>
v1.1 BOM, Assembly Drawing actualized
</commit_message>
<xml_diff>
--- a/pcb/v1.1/jumpers_map.xlsx
+++ b/pcb/v1.1/jumpers_map.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Work\auto_informer\board\pcb\v1.1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEB2541-CDE0-4A29-9EE3-EDA28745F405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19275" yWindow="2535" windowWidth="17820" windowHeight="10590"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Позиционное обозначение</t>
   </si>
@@ -78,9 +84,6 @@
     <t>R68</t>
   </si>
   <si>
-    <t>Подключенbе "-" аккумулятора к GND в отсутстсвие VT4</t>
-  </si>
-  <si>
     <t>Примечание</t>
   </si>
   <si>
@@ -123,12 +126,6 @@
     <t>Pull-up кнопок к 1.8V (MPU)</t>
   </si>
   <si>
-    <t>Pull-up кнопок к 3.3V (MCU)</t>
-  </si>
-  <si>
-    <t>Подключение сигнала микрофона при отсутствии штекера к AGND</t>
-  </si>
-  <si>
     <t>Задает коэф. Умножителя частоты D7</t>
   </si>
   <si>
@@ -154,13 +151,22 @@
   </si>
   <si>
     <t>TDA2003V</t>
+  </si>
+  <si>
+    <t>Подключение "-" аккумулятора к GND в отсутстсвие VT4</t>
+  </si>
+  <si>
+    <t>Подключение сигнала микрофона к AGND при отсутствии штекера</t>
+  </si>
+  <si>
+    <t>Pull-up кнопок к 3.3V (MCU) - не используется</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,29 +503,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" customWidth="1"/>
+    <col min="4" max="5" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:5" ht="32.25" customHeight="1" thickBot="1">
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -530,264 +536,268 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1">
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="2:5" ht="45.75" thickBot="1">
+    <row r="7" spans="2:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="30.75" thickBot="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="2:5" ht="15.75" thickBot="1">
+    <row r="9" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1">
+    <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:5" ht="15.75" thickBot="1">
+    <row r="13" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:5" ht="15.75" thickBot="1">
+    <row r="15" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1">
+    <row r="17" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1">
+    <row r="19" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" ht="30.75" thickBot="1">
+    <row r="23" spans="2:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="2:5" ht="30.75" thickBot="1">
-      <c r="B24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="2:5" ht="15.75" thickBot="1">
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1">
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>

</xml_diff>